<commit_message>
Adding Test for RegistrationPage
</commit_message>
<xml_diff>
--- a/data/pet-store-data.xlsx
+++ b/data/pet-store-data.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{988A31BE-7465-4334-89A6-CBD04210EBE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="20115" windowHeight="13680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cart_items" sheetId="1" r:id="rId1"/>
     <sheet name="users" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:H10"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="615">
   <si>
     <t>ITEM_ID</t>
   </si>
@@ -23,9 +25,6 @@
     <t>ITEM_LINK</t>
   </si>
   <si>
-    <t>User ID</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
@@ -1410,13 +1409,467 @@
   </si>
   <si>
     <t>https://petstore.octoperf.com/actions/Catalog.action?viewItem=&amp;itemId=EST-13</t>
+  </si>
+  <si>
+    <t>61c28</t>
+  </si>
+  <si>
+    <t>33aea</t>
+  </si>
+  <si>
+    <t>1dfdc</t>
+  </si>
+  <si>
+    <t>0981e</t>
+  </si>
+  <si>
+    <t>7304d</t>
+  </si>
+  <si>
+    <t>2c116</t>
+  </si>
+  <si>
+    <t>dd3c1</t>
+  </si>
+  <si>
+    <t>9abfa</t>
+  </si>
+  <si>
+    <t>e2447</t>
+  </si>
+  <si>
+    <t>b1b73</t>
+  </si>
+  <si>
+    <t>ab663</t>
+  </si>
+  <si>
+    <t>b350d</t>
+  </si>
+  <si>
+    <t>1dd90</t>
+  </si>
+  <si>
+    <t>cb275</t>
+  </si>
+  <si>
+    <t>613e0</t>
+  </si>
+  <si>
+    <t>93cff</t>
+  </si>
+  <si>
+    <t>af10d</t>
+  </si>
+  <si>
+    <t>97191</t>
+  </si>
+  <si>
+    <t>0b93b</t>
+  </si>
+  <si>
+    <t>41613</t>
+  </si>
+  <si>
+    <t>4e3e5</t>
+  </si>
+  <si>
+    <t>68995</t>
+  </si>
+  <si>
+    <t>23517</t>
+  </si>
+  <si>
+    <t>e8136</t>
+  </si>
+  <si>
+    <t>0ed1c</t>
+  </si>
+  <si>
+    <t>ae2e5</t>
+  </si>
+  <si>
+    <t>e93bc</t>
+  </si>
+  <si>
+    <t>ae27c</t>
+  </si>
+  <si>
+    <t>22e19</t>
+  </si>
+  <si>
+    <t>264a5</t>
+  </si>
+  <si>
+    <t>c11f8</t>
+  </si>
+  <si>
+    <t>54439</t>
+  </si>
+  <si>
+    <t>75fa3</t>
+  </si>
+  <si>
+    <t>21875</t>
+  </si>
+  <si>
+    <t>853a3</t>
+  </si>
+  <si>
+    <t>b02ea</t>
+  </si>
+  <si>
+    <t>2f578</t>
+  </si>
+  <si>
+    <t>8229d</t>
+  </si>
+  <si>
+    <t>81996</t>
+  </si>
+  <si>
+    <t>5ce18</t>
+  </si>
+  <si>
+    <t>37c73</t>
+  </si>
+  <si>
+    <t>c238b</t>
+  </si>
+  <si>
+    <t>722df</t>
+  </si>
+  <si>
+    <t>c85f0</t>
+  </si>
+  <si>
+    <t>33051</t>
+  </si>
+  <si>
+    <t>0fae5</t>
+  </si>
+  <si>
+    <t>838cf</t>
+  </si>
+  <si>
+    <t>0df35</t>
+  </si>
+  <si>
+    <t>2d8e9</t>
+  </si>
+  <si>
+    <t>ed274</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>b74d29</t>
+  </si>
+  <si>
+    <t>abe1d2</t>
+  </si>
+  <si>
+    <t>ec328b</t>
+  </si>
+  <si>
+    <t>eb6c35</t>
+  </si>
+  <si>
+    <t>fd35f6</t>
+  </si>
+  <si>
+    <t>85a259</t>
+  </si>
+  <si>
+    <t>e7139e</t>
+  </si>
+  <si>
+    <t>a9d7f1</t>
+  </si>
+  <si>
+    <t>3d03d2</t>
+  </si>
+  <si>
+    <t>338519</t>
+  </si>
+  <si>
+    <t>9088eb</t>
+  </si>
+  <si>
+    <t>97ad86</t>
+  </si>
+  <si>
+    <t>b59715</t>
+  </si>
+  <si>
+    <t>5e8aeb</t>
+  </si>
+  <si>
+    <t>b6cc38</t>
+  </si>
+  <si>
+    <t>94e901</t>
+  </si>
+  <si>
+    <t>19fe01</t>
+  </si>
+  <si>
+    <t>b3fe19</t>
+  </si>
+  <si>
+    <t>d7d23a</t>
+  </si>
+  <si>
+    <t>879555</t>
+  </si>
+  <si>
+    <t>baa53a</t>
+  </si>
+  <si>
+    <t>4eb770</t>
+  </si>
+  <si>
+    <t>2dccc8</t>
+  </si>
+  <si>
+    <t>eda27a</t>
+  </si>
+  <si>
+    <t>a79e28</t>
+  </si>
+  <si>
+    <t>051aaf</t>
+  </si>
+  <si>
+    <t>f3e00c</t>
+  </si>
+  <si>
+    <t>daa81f</t>
+  </si>
+  <si>
+    <t>6bf61c</t>
+  </si>
+  <si>
+    <t>2d7ea7</t>
+  </si>
+  <si>
+    <t>e28783</t>
+  </si>
+  <si>
+    <t>275854</t>
+  </si>
+  <si>
+    <t>89f656</t>
+  </si>
+  <si>
+    <t>575962</t>
+  </si>
+  <si>
+    <t>63990a</t>
+  </si>
+  <si>
+    <t>a53584</t>
+  </si>
+  <si>
+    <t>5649fb</t>
+  </si>
+  <si>
+    <t>53077f</t>
+  </si>
+  <si>
+    <t>e4dbc8</t>
+  </si>
+  <si>
+    <t>57b0c1</t>
+  </si>
+  <si>
+    <t>8f4467</t>
+  </si>
+  <si>
+    <t>c5503e</t>
+  </si>
+  <si>
+    <t>60548b</t>
+  </si>
+  <si>
+    <t>09cb8b</t>
+  </si>
+  <si>
+    <t>eb3085</t>
+  </si>
+  <si>
+    <t>77bbc3</t>
+  </si>
+  <si>
+    <t>f59058</t>
+  </si>
+  <si>
+    <t>6ebf47</t>
+  </si>
+  <si>
+    <t>d88619</t>
+  </si>
+  <si>
+    <t>d44a83</t>
+  </si>
+  <si>
+    <t>56b62f</t>
+  </si>
+  <si>
+    <t>d51c34</t>
+  </si>
+  <si>
+    <t>b0c995</t>
+  </si>
+  <si>
+    <t>838d29</t>
+  </si>
+  <si>
+    <t>e599db</t>
+  </si>
+  <si>
+    <t>b227d8</t>
+  </si>
+  <si>
+    <t>7fb0f4</t>
+  </si>
+  <si>
+    <t>087e9d</t>
+  </si>
+  <si>
+    <t>945fdd</t>
+  </si>
+  <si>
+    <t>622948</t>
+  </si>
+  <si>
+    <t>7e7b41</t>
+  </si>
+  <si>
+    <t>482fb9</t>
+  </si>
+  <si>
+    <t>b601cc</t>
+  </si>
+  <si>
+    <t>b4292a</t>
+  </si>
+  <si>
+    <t>c8a1fa</t>
+  </si>
+  <si>
+    <t>85ff05</t>
+  </si>
+  <si>
+    <t>92243f</t>
+  </si>
+  <si>
+    <t>34258f</t>
+  </si>
+  <si>
+    <t>1aec88</t>
+  </si>
+  <si>
+    <t>c68e82</t>
+  </si>
+  <si>
+    <t>28889d</t>
+  </si>
+  <si>
+    <t>ef412a</t>
+  </si>
+  <si>
+    <t>c7abd6</t>
+  </si>
+  <si>
+    <t>d8011c</t>
+  </si>
+  <si>
+    <t>4cf789</t>
+  </si>
+  <si>
+    <t>f009a3</t>
+  </si>
+  <si>
+    <t>516c03</t>
+  </si>
+  <si>
+    <t>407e8c</t>
+  </si>
+  <si>
+    <t>99b08f</t>
+  </si>
+  <si>
+    <t>02237b</t>
+  </si>
+  <si>
+    <t>09b5dc</t>
+  </si>
+  <si>
+    <t>594516</t>
+  </si>
+  <si>
+    <t>68528c</t>
+  </si>
+  <si>
+    <t>16ffc8</t>
+  </si>
+  <si>
+    <t>4159f2</t>
+  </si>
+  <si>
+    <t>c74fa5</t>
+  </si>
+  <si>
+    <t>a3e086</t>
+  </si>
+  <si>
+    <t>a6615e</t>
+  </si>
+  <si>
+    <t>a36d3e</t>
+  </si>
+  <si>
+    <t>03554d</t>
+  </si>
+  <si>
+    <t>cec4e1</t>
+  </si>
+  <si>
+    <t>f00e8a</t>
+  </si>
+  <si>
+    <t>41ea64</t>
+  </si>
+  <si>
+    <t>118246</t>
+  </si>
+  <si>
+    <t>fadd3d</t>
+  </si>
+  <si>
+    <t>0705c8</t>
+  </si>
+  <si>
+    <t>4d19f4</t>
+  </si>
+  <si>
+    <t>2ce623</t>
+  </si>
+  <si>
+    <t>211f57</t>
+  </si>
+  <si>
+    <t>b01e31</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1583,6 +2036,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1629,7 +2090,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1661,9 +2122,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1695,6 +2174,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1870,20 +2367,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="108" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="28.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="108.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1891,2056 +2388,2056 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
+        <v>444</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>445</v>
       </c>
-      <c r="B2" s="13" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="12" t="s">
+      <c r="B3" s="13" t="s">
         <v>447</v>
       </c>
-      <c r="B3" s="13" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="12" t="s">
+      <c r="B4" s="13" t="s">
         <v>449</v>
       </c>
-      <c r="B4" s="13" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>451</v>
+      </c>
+      <c r="B5" s="13" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="12" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="B6" s="13" t="s">
         <v>452</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="12" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
         <v>454</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="12" t="s">
+      <c r="B7" s="13" t="s">
         <v>455</v>
       </c>
-      <c r="B7" s="13" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>457</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="12" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>459</v>
+      </c>
+      <c r="B9" s="13" t="s">
         <v>458</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="12" t="s">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>461</v>
+      </c>
+      <c r="B10" s="13" t="s">
         <v>460</v>
       </c>
-      <c r="B9" s="13" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="12" t="s">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
         <v>462</v>
       </c>
-      <c r="B10" s="13" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="12" t="s">
+      <c r="B11" s="13" t="s">
         <v>463</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>464</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
-    <hyperlink ref="B8" r:id="rId7"/>
-    <hyperlink ref="B9" r:id="rId8"/>
-    <hyperlink ref="B10" r:id="rId9"/>
-    <hyperlink ref="B11" r:id="rId10"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="17.28515625" style="3"/>
-    <col min="5" max="5" width="25.85546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" style="3"/>
-    <col min="7" max="7" width="27.42578125" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="17.28515625" style="3"/>
+    <col min="1" max="4" style="3" width="17.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="3" width="25.85546875" collapsed="true"/>
+    <col min="6" max="6" style="3" width="17.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="3" width="27.42578125" collapsed="true"/>
+    <col min="8" max="16384" style="3" width="17.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30.75" thickBot="1">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>565</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="8" t="s">
         <v>21</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>22</v>
       </c>
       <c r="K2" s="9">
         <v>33101</v>
       </c>
       <c r="L2" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>566</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="J3" s="8" t="s">
         <v>31</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>32</v>
       </c>
       <c r="K3" s="9">
         <v>23308</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A4" s="7">
-        <v>3</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>567</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="F4" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="G4" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="H4" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="I4" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="J4" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>41</v>
       </c>
       <c r="K4" s="9">
         <v>26739</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A5" s="4">
-        <v>4</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>568</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="E5" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="H5" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="I5" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="J5" s="8" t="s">
         <v>49</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>50</v>
       </c>
       <c r="K5" s="9">
         <v>74468</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A6" s="4">
-        <v>5</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>569</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="F6" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="H6" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="I6" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="J6" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>59</v>
       </c>
       <c r="K6" s="9">
         <v>28160</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A7" s="7">
-        <v>6</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>570</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="E7" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="F7" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="G7" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="H7" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="I7" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="J7" s="8" t="s">
         <v>67</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>68</v>
       </c>
       <c r="K7" s="9">
         <v>15545</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A8" s="4">
-        <v>7</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>571</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="D8" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="E8" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="F8" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="G8" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="H8" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="I8" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="J8" s="8" t="s">
         <v>76</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>77</v>
       </c>
       <c r="K8" s="9">
         <v>65080</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A9" s="4">
-        <v>8</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>572</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="D9" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="E9" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="F9" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="G9" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="H9" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="I9" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="J9" s="8" t="s">
         <v>85</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>86</v>
       </c>
       <c r="K9" s="9">
         <v>82718</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A10" s="7">
-        <v>9</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>573</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="D10" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="E10" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="F10" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="G10" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="H10" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="I10" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="J10" s="8" t="s">
         <v>94</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>95</v>
       </c>
       <c r="K10" s="9">
         <v>10273</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A11" s="4">
-        <v>10</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>574</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="D11" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="E11" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="F11" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="G11" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="H11" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="I11" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="J11" s="8" t="s">
         <v>103</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>104</v>
       </c>
       <c r="K11" s="9">
         <v>58651</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A12" s="4">
-        <v>11</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>575</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="D12" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="E12" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="F12" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="G12" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="H12" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="I12" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="J12" s="8" t="s">
         <v>112</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>113</v>
       </c>
       <c r="K12" s="9">
         <v>46851</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A13" s="7">
-        <v>12</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>576</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="D13" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="E13" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="F13" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="G13" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="H13" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="I13" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="J13" s="8" t="s">
         <v>121</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>122</v>
       </c>
       <c r="K13" s="9">
         <v>15601</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A14" s="4">
-        <v>13</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>577</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="D14" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="E14" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="F14" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="G14" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="H14" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="I14" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="I14" s="5" t="s">
-        <v>130</v>
-      </c>
       <c r="J14" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K14" s="9">
         <v>47992</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A15" s="4">
-        <v>14</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>578</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="D15" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="E15" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="F15" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="G15" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="H15" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="I15" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="I15" s="5" t="s">
-        <v>138</v>
-      </c>
       <c r="J15" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K15" s="9">
         <v>78338</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A16" s="7">
-        <v>15</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>579</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="D16" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="E16" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="F16" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="G16" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="H16" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="I16" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="I16" s="5" t="s">
+      <c r="J16" s="8" t="s">
         <v>146</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>147</v>
       </c>
       <c r="K16" s="9">
         <v>76465</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A17" s="4">
-        <v>16</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>580</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="D17" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="E17" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="F17" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="G17" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="H17" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="I17" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="I17" s="5" t="s">
-        <v>155</v>
-      </c>
       <c r="J17" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K17" s="9">
         <v>38369</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A18" s="4">
-        <v>17</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>581</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="D18" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="E18" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="F18" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="G18" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="H18" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="H18" s="6" t="s">
+      <c r="I18" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="I18" s="5" t="s">
+      <c r="J18" s="8" t="s">
         <v>163</v>
-      </c>
-      <c r="J18" s="8" t="s">
-        <v>164</v>
       </c>
       <c r="K18" s="9">
         <v>18449</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A19" s="7">
-        <v>18</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>582</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="D19" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="E19" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="F19" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="G19" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="H19" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="H19" s="6" t="s">
+      <c r="I19" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="I19" s="5" t="s">
-        <v>172</v>
-      </c>
       <c r="J19" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K19" s="9">
         <v>52640</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A20" s="4">
-        <v>19</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>583</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="D20" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="E20" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="F20" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="G20" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="H20" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="I20" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="I20" s="5" t="s">
-        <v>180</v>
-      </c>
       <c r="J20" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K20" s="9">
         <v>15250</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A21" s="4">
-        <v>20</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>584</v>
       </c>
       <c r="B21" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="D21" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="E21" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="F21" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="G21" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="H21" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="H21" s="6" t="s">
+      <c r="I21" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="I21" s="5" t="s">
+      <c r="J21" s="8" t="s">
         <v>188</v>
-      </c>
-      <c r="J21" s="8" t="s">
-        <v>189</v>
       </c>
       <c r="K21" s="9">
         <v>93718</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A22" s="7">
-        <v>21</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
+        <v>585</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="D22" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="E22" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="F22" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="G22" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="G22" s="6" t="s">
+      <c r="H22" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="H22" s="6" t="s">
+      <c r="I22" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="I22" s="5" t="s">
+      <c r="J22" s="8" t="s">
         <v>197</v>
-      </c>
-      <c r="J22" s="8" t="s">
-        <v>198</v>
       </c>
       <c r="K22" s="9">
         <v>56016</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A23" s="4">
-        <v>22</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>586</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="D23" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="E23" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="F23" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="G23" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="G23" s="6" t="s">
+      <c r="H23" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="H23" s="6" t="s">
+      <c r="I23" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="I23" s="5" t="s">
-        <v>206</v>
-      </c>
       <c r="J23" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K23" s="9">
         <v>45222</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A24" s="4">
-        <v>23</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>587</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="D24" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="E24" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="F24" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="G24" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="G24" s="6" t="s">
+      <c r="H24" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="H24" s="6" t="s">
+      <c r="I24" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="I24" s="5" t="s">
+      <c r="J24" s="8" t="s">
         <v>214</v>
-      </c>
-      <c r="J24" s="8" t="s">
-        <v>215</v>
       </c>
       <c r="K24" s="9">
         <v>10597</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A25" s="7">
-        <v>24</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
+        <v>588</v>
       </c>
       <c r="B25" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="D25" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="E25" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="F25" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="G25" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="G25" s="6" t="s">
+      <c r="H25" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="H25" s="6" t="s">
+      <c r="I25" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="I25" s="5" t="s">
+      <c r="J25" s="8" t="s">
         <v>223</v>
-      </c>
-      <c r="J25" s="8" t="s">
-        <v>224</v>
       </c>
       <c r="K25" s="9">
         <v>39581</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A26" s="4">
-        <v>25</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>589</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="D26" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="E26" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="F26" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="G26" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="G26" s="6" t="s">
+      <c r="H26" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="H26" s="6" t="s">
+      <c r="I26" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="I26" s="5" t="s">
+      <c r="J26" s="8" t="s">
         <v>232</v>
-      </c>
-      <c r="J26" s="8" t="s">
-        <v>233</v>
       </c>
       <c r="K26" s="9">
         <v>5069</v>
       </c>
       <c r="L26" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A27" s="4">
-        <v>26</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>590</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="D27" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="E27" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="F27" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="G27" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="H27" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="H27" s="6" t="s">
+      <c r="I27" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="I27" s="5" t="s">
+      <c r="J27" s="8" t="s">
         <v>241</v>
-      </c>
-      <c r="J27" s="8" t="s">
-        <v>242</v>
       </c>
       <c r="K27" s="9">
         <v>28723</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A28" s="7">
-        <v>27</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>591</v>
       </c>
       <c r="B28" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="D28" s="6" t="s">
         <v>244</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="E28" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="F28" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="F28" s="6" t="s">
+      <c r="G28" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="G28" s="6" t="s">
+      <c r="H28" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="H28" s="6" t="s">
+      <c r="I28" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="I28" s="5" t="s">
-        <v>250</v>
-      </c>
       <c r="J28" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K28" s="9">
         <v>38478</v>
       </c>
       <c r="L28" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A29" s="4">
-        <v>28</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>592</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="D29" s="6" t="s">
         <v>252</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="E29" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="E29" s="10" t="s">
+      <c r="F29" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="F29" s="6" t="s">
+      <c r="G29" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="G29" s="6" t="s">
+      <c r="H29" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="H29" s="6" t="s">
+      <c r="I29" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="I29" s="5" t="s">
-        <v>258</v>
-      </c>
       <c r="J29" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K29" s="9">
         <v>28144</v>
       </c>
       <c r="L29" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A30" s="4">
-        <v>29</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>593</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="C30" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="D30" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="E30" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="F30" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="F30" s="6" t="s">
+      <c r="G30" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="G30" s="6" t="s">
+      <c r="H30" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="H30" s="6" t="s">
+      <c r="I30" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="I30" s="5" t="s">
+      <c r="J30" s="8" t="s">
         <v>266</v>
-      </c>
-      <c r="J30" s="8" t="s">
-        <v>267</v>
       </c>
       <c r="K30" s="9">
         <v>40062</v>
       </c>
       <c r="L30" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A31" s="7">
-        <v>30</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>594</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="C31" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="D31" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="E31" s="7" t="s">
         <v>270</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="F31" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="F31" s="6" t="s">
+      <c r="G31" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="G31" s="6" t="s">
+      <c r="H31" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="H31" s="6" t="s">
+      <c r="I31" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="I31" s="5" t="s">
-        <v>275</v>
-      </c>
       <c r="J31" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K31" s="9">
         <v>35073</v>
       </c>
       <c r="L31" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A32" s="4">
-        <v>31</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>595</v>
       </c>
       <c r="B32" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="C32" s="6" t="s">
         <v>276</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="D32" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="E32" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="E32" s="7" t="s">
+      <c r="F32" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="F32" s="6" t="s">
+      <c r="G32" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="G32" s="6" t="s">
+      <c r="H32" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="H32" s="6" t="s">
+      <c r="I32" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="I32" s="5" t="s">
-        <v>283</v>
-      </c>
       <c r="J32" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K32" s="9">
         <v>24464</v>
       </c>
       <c r="L32" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A33" s="4">
-        <v>32</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>596</v>
       </c>
       <c r="B33" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="C33" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="D33" s="6" t="s">
         <v>285</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="E33" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="F33" s="6" t="s">
         <v>287</v>
       </c>
-      <c r="F33" s="6" t="s">
+      <c r="G33" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="G33" s="6" t="s">
+      <c r="H33" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="H33" s="6" t="s">
+      <c r="I33" s="5" t="s">
         <v>290</v>
       </c>
-      <c r="I33" s="5" t="s">
-        <v>291</v>
-      </c>
       <c r="J33" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K33" s="9">
         <v>19529</v>
       </c>
       <c r="L33" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A34" s="7">
-        <v>33</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>597</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C34" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="D34" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="E34" s="7" t="s">
         <v>294</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="F34" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="F34" s="6" t="s">
+      <c r="G34" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="G34" s="6" t="s">
+      <c r="H34" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="H34" s="6" t="s">
+      <c r="I34" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="I34" s="5" t="s">
+      <c r="J34" s="8" t="s">
         <v>299</v>
-      </c>
-      <c r="J34" s="8" t="s">
-        <v>300</v>
       </c>
       <c r="K34" s="9">
         <v>44645</v>
       </c>
       <c r="L34" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A35" s="4">
-        <v>34</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>598</v>
       </c>
       <c r="B35" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="C35" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="D35" s="6" t="s">
         <v>302</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="E35" s="7" t="s">
         <v>303</v>
       </c>
-      <c r="E35" s="7" t="s">
+      <c r="F35" s="6" t="s">
         <v>304</v>
       </c>
-      <c r="F35" s="6" t="s">
+      <c r="G35" s="6" t="s">
         <v>305</v>
       </c>
-      <c r="G35" s="6" t="s">
+      <c r="H35" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="H35" s="6" t="s">
+      <c r="I35" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="I35" s="5" t="s">
+      <c r="J35" s="8" t="s">
         <v>308</v>
-      </c>
-      <c r="J35" s="8" t="s">
-        <v>309</v>
       </c>
       <c r="K35" s="9">
         <v>95120</v>
       </c>
       <c r="L35" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A36" s="4">
-        <v>35</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>599</v>
       </c>
       <c r="B36" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="C36" s="6" t="s">
         <v>310</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="D36" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="E36" s="7" t="s">
         <v>312</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="F36" s="6" t="s">
         <v>313</v>
       </c>
-      <c r="F36" s="6" t="s">
+      <c r="G36" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="G36" s="6" t="s">
+      <c r="H36" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="H36" s="6" t="s">
+      <c r="I36" s="5" t="s">
         <v>316</v>
       </c>
-      <c r="I36" s="5" t="s">
+      <c r="J36" s="8" t="s">
         <v>317</v>
-      </c>
-      <c r="J36" s="8" t="s">
-        <v>318</v>
       </c>
       <c r="K36" s="9">
         <v>43548</v>
       </c>
       <c r="L36" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A37" s="7">
-        <v>36</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
+        <v>600</v>
       </c>
       <c r="B37" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C37" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="D37" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="E37" s="7" t="s">
         <v>321</v>
       </c>
-      <c r="E37" s="7" t="s">
+      <c r="F37" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="F37" s="6" t="s">
+      <c r="G37" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="G37" s="6" t="s">
+      <c r="H37" s="6" t="s">
         <v>324</v>
       </c>
-      <c r="H37" s="6" t="s">
+      <c r="I37" s="5" t="s">
         <v>325</v>
       </c>
-      <c r="I37" s="5" t="s">
-        <v>326</v>
-      </c>
       <c r="J37" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K37" s="9">
         <v>31790</v>
       </c>
       <c r="L37" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A38" s="4">
-        <v>37</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>601</v>
       </c>
       <c r="B38" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="C38" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="D38" s="6" t="s">
         <v>328</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="E38" s="7" t="s">
         <v>329</v>
       </c>
-      <c r="E38" s="7" t="s">
+      <c r="F38" s="6" t="s">
         <v>330</v>
       </c>
-      <c r="F38" s="6" t="s">
+      <c r="G38" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="G38" s="6" t="s">
+      <c r="H38" s="6" t="s">
         <v>332</v>
       </c>
-      <c r="H38" s="6" t="s">
+      <c r="I38" s="5" t="s">
         <v>333</v>
       </c>
-      <c r="I38" s="5" t="s">
+      <c r="J38" s="8" t="s">
         <v>334</v>
-      </c>
-      <c r="J38" s="8" t="s">
-        <v>335</v>
       </c>
       <c r="K38" s="9">
         <v>11531</v>
       </c>
       <c r="L38" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A39" s="4">
-        <v>38</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>602</v>
       </c>
       <c r="B39" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="C39" s="6" t="s">
         <v>336</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="D39" s="6" t="s">
         <v>337</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="E39" s="7" t="s">
         <v>338</v>
       </c>
-      <c r="E39" s="7" t="s">
+      <c r="F39" s="6" t="s">
         <v>339</v>
       </c>
-      <c r="F39" s="6" t="s">
+      <c r="G39" s="6" t="s">
         <v>340</v>
       </c>
-      <c r="G39" s="6" t="s">
+      <c r="H39" s="6" t="s">
         <v>341</v>
       </c>
-      <c r="H39" s="6" t="s">
+      <c r="I39" s="5" t="s">
         <v>342</v>
       </c>
-      <c r="I39" s="5" t="s">
-        <v>343</v>
-      </c>
       <c r="J39" s="8" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="K39" s="9">
         <v>61468</v>
       </c>
       <c r="L39" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A40" s="7">
-        <v>39</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
+        <v>603</v>
       </c>
       <c r="B40" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="C40" s="6" t="s">
         <v>344</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="D40" s="6" t="s">
         <v>345</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="E40" s="7" t="s">
         <v>346</v>
       </c>
-      <c r="E40" s="7" t="s">
+      <c r="F40" s="6" t="s">
         <v>347</v>
       </c>
-      <c r="F40" s="6" t="s">
+      <c r="G40" s="6" t="s">
         <v>348</v>
       </c>
-      <c r="G40" s="6" t="s">
+      <c r="H40" s="6" t="s">
         <v>349</v>
       </c>
-      <c r="H40" s="6" t="s">
+      <c r="I40" s="5" t="s">
         <v>350</v>
       </c>
-      <c r="I40" s="5" t="s">
-        <v>351</v>
-      </c>
       <c r="J40" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K40" s="9">
         <v>20223</v>
       </c>
       <c r="L40" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A41" s="4">
-        <v>40</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>604</v>
       </c>
       <c r="B41" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="C41" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="D41" s="6" t="s">
         <v>353</v>
       </c>
-      <c r="D41" s="6" t="s">
+      <c r="E41" s="7" t="s">
         <v>354</v>
       </c>
-      <c r="E41" s="7" t="s">
+      <c r="F41" s="6" t="s">
         <v>355</v>
       </c>
-      <c r="F41" s="6" t="s">
+      <c r="G41" s="6" t="s">
         <v>356</v>
       </c>
-      <c r="G41" s="6" t="s">
+      <c r="H41" s="6" t="s">
         <v>357</v>
       </c>
-      <c r="H41" s="6" t="s">
+      <c r="I41" s="5" t="s">
         <v>358</v>
       </c>
-      <c r="I41" s="5" t="s">
-        <v>359</v>
-      </c>
       <c r="J41" s="8" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K41" s="9">
         <v>48636</v>
       </c>
       <c r="L41" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A42" s="4">
-        <v>41</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>605</v>
       </c>
       <c r="B42" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="C42" s="6" t="s">
         <v>360</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="D42" s="6" t="s">
         <v>361</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="E42" s="7" t="s">
         <v>362</v>
       </c>
-      <c r="E42" s="7" t="s">
+      <c r="F42" s="6" t="s">
         <v>363</v>
       </c>
-      <c r="F42" s="6" t="s">
+      <c r="G42" s="6" t="s">
         <v>364</v>
       </c>
-      <c r="G42" s="6" t="s">
+      <c r="H42" s="6" t="s">
         <v>365</v>
       </c>
-      <c r="H42" s="6" t="s">
+      <c r="I42" s="5" t="s">
         <v>366</v>
       </c>
-      <c r="I42" s="5" t="s">
-        <v>367</v>
-      </c>
       <c r="J42" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K42" s="9">
         <v>30140</v>
       </c>
       <c r="L42" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A43" s="7">
-        <v>42</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>606</v>
       </c>
       <c r="B43" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="C43" s="6" t="s">
         <v>368</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="D43" s="6" t="s">
         <v>369</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="E43" s="7" t="s">
         <v>370</v>
       </c>
-      <c r="E43" s="7" t="s">
+      <c r="F43" s="6" t="s">
         <v>371</v>
       </c>
-      <c r="F43" s="6" t="s">
+      <c r="G43" s="6" t="s">
         <v>372</v>
       </c>
-      <c r="G43" s="6" t="s">
+      <c r="H43" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="H43" s="6" t="s">
+      <c r="I43" s="5" t="s">
         <v>374</v>
       </c>
-      <c r="I43" s="5" t="s">
+      <c r="J43" s="8" t="s">
         <v>375</v>
-      </c>
-      <c r="J43" s="8" t="s">
-        <v>376</v>
       </c>
       <c r="K43" s="9">
         <v>85381</v>
       </c>
       <c r="L43" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A44" s="4">
-        <v>43</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>607</v>
       </c>
       <c r="B44" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="C44" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="D44" s="6" t="s">
         <v>378</v>
       </c>
-      <c r="D44" s="6" t="s">
+      <c r="E44" s="10" t="s">
         <v>379</v>
       </c>
-      <c r="E44" s="10" t="s">
+      <c r="F44" s="6" t="s">
         <v>380</v>
       </c>
-      <c r="F44" s="6" t="s">
+      <c r="G44" s="6" t="s">
         <v>381</v>
       </c>
-      <c r="G44" s="6" t="s">
+      <c r="H44" s="6" t="s">
         <v>382</v>
       </c>
-      <c r="H44" s="6" t="s">
+      <c r="I44" s="5" t="s">
         <v>383</v>
       </c>
-      <c r="I44" s="5" t="s">
+      <c r="J44" s="8" t="s">
         <v>384</v>
-      </c>
-      <c r="J44" s="8" t="s">
-        <v>385</v>
       </c>
       <c r="K44" s="9">
         <v>57073</v>
       </c>
       <c r="L44" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A45" s="4">
-        <v>44</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>608</v>
       </c>
       <c r="B45" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="C45" s="6" t="s">
         <v>386</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="D45" s="6" t="s">
         <v>387</v>
       </c>
-      <c r="D45" s="6" t="s">
+      <c r="E45" s="7" t="s">
         <v>388</v>
       </c>
-      <c r="E45" s="7" t="s">
+      <c r="F45" s="6" t="s">
         <v>389</v>
       </c>
-      <c r="F45" s="6" t="s">
+      <c r="G45" s="6" t="s">
         <v>390</v>
       </c>
-      <c r="G45" s="6" t="s">
+      <c r="H45" s="6" t="s">
         <v>391</v>
       </c>
-      <c r="H45" s="6" t="s">
+      <c r="I45" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J45" s="8" t="s">
         <v>392</v>
-      </c>
-      <c r="I45" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J45" s="8" t="s">
-        <v>393</v>
       </c>
       <c r="K45" s="9">
         <v>65612</v>
       </c>
       <c r="L45" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A46" s="7">
-        <v>45</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
+        <v>609</v>
       </c>
       <c r="B46" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="C46" s="6" t="s">
         <v>394</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="D46" s="6" t="s">
         <v>395</v>
       </c>
-      <c r="D46" s="6" t="s">
+      <c r="E46" s="7" t="s">
         <v>396</v>
       </c>
-      <c r="E46" s="7" t="s">
+      <c r="F46" s="6" t="s">
         <v>397</v>
       </c>
-      <c r="F46" s="6" t="s">
+      <c r="G46" s="6" t="s">
         <v>398</v>
       </c>
-      <c r="G46" s="6" t="s">
+      <c r="H46" s="6" t="s">
         <v>399</v>
       </c>
-      <c r="H46" s="6" t="s">
+      <c r="I46" s="5" t="s">
         <v>400</v>
       </c>
-      <c r="I46" s="5" t="s">
-        <v>401</v>
-      </c>
       <c r="J46" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K46" s="9">
         <v>67448</v>
       </c>
       <c r="L46" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A47" s="4">
-        <v>46</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>610</v>
       </c>
       <c r="B47" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="C47" s="6" t="s">
         <v>402</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="D47" s="6" t="s">
         <v>403</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="E47" s="7" t="s">
         <v>404</v>
       </c>
-      <c r="E47" s="7" t="s">
+      <c r="F47" s="6" t="s">
         <v>405</v>
       </c>
-      <c r="F47" s="6" t="s">
+      <c r="G47" s="6" t="s">
         <v>406</v>
       </c>
-      <c r="G47" s="6" t="s">
+      <c r="H47" s="6" t="s">
         <v>407</v>
       </c>
-      <c r="H47" s="6" t="s">
+      <c r="I47" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="I47" s="5" t="s">
-        <v>409</v>
-      </c>
       <c r="J47" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K47" s="9">
         <v>59405</v>
       </c>
       <c r="L47" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A48" s="4">
-        <v>47</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>611</v>
       </c>
       <c r="B48" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="C48" s="6" t="s">
         <v>410</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="D48" s="6" t="s">
         <v>411</v>
       </c>
-      <c r="D48" s="6" t="s">
+      <c r="E48" s="7" t="s">
         <v>412</v>
       </c>
-      <c r="E48" s="7" t="s">
+      <c r="F48" s="6" t="s">
         <v>413</v>
       </c>
-      <c r="F48" s="6" t="s">
+      <c r="G48" s="6" t="s">
         <v>414</v>
       </c>
-      <c r="G48" s="6" t="s">
+      <c r="H48" s="6" t="s">
         <v>415</v>
       </c>
-      <c r="H48" s="6" t="s">
+      <c r="I48" s="5" t="s">
         <v>416</v>
       </c>
-      <c r="I48" s="5" t="s">
-        <v>417</v>
-      </c>
       <c r="J48" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K48" s="9">
         <v>92563</v>
       </c>
       <c r="L48" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A49" s="7">
-        <v>48</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="7" t="s">
+        <v>612</v>
       </c>
       <c r="B49" s="5" t="s">
+        <v>417</v>
+      </c>
+      <c r="C49" s="6" t="s">
         <v>418</v>
       </c>
-      <c r="C49" s="6" t="s">
+      <c r="D49" s="6" t="s">
         <v>419</v>
       </c>
-      <c r="D49" s="6" t="s">
+      <c r="E49" s="7" t="s">
         <v>420</v>
       </c>
-      <c r="E49" s="7" t="s">
+      <c r="F49" s="6" t="s">
         <v>421</v>
       </c>
-      <c r="F49" s="6" t="s">
+      <c r="G49" s="6" t="s">
         <v>422</v>
       </c>
-      <c r="G49" s="6" t="s">
+      <c r="H49" s="6" t="s">
         <v>423</v>
       </c>
-      <c r="H49" s="6" t="s">
+      <c r="I49" s="5" t="s">
         <v>424</v>
       </c>
-      <c r="I49" s="5" t="s">
+      <c r="J49" s="8" t="s">
         <v>425</v>
-      </c>
-      <c r="J49" s="8" t="s">
-        <v>426</v>
       </c>
       <c r="K49" s="9">
         <v>94271</v>
       </c>
       <c r="L49" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A50" s="4">
-        <v>49</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>613</v>
       </c>
       <c r="B50" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="C50" s="6" t="s">
         <v>427</v>
       </c>
-      <c r="C50" s="6" t="s">
+      <c r="D50" s="6" t="s">
         <v>428</v>
       </c>
-      <c r="D50" s="6" t="s">
+      <c r="E50" s="7" t="s">
         <v>429</v>
       </c>
-      <c r="E50" s="7" t="s">
+      <c r="F50" s="6" t="s">
         <v>430</v>
       </c>
-      <c r="F50" s="6" t="s">
+      <c r="G50" s="6" t="s">
         <v>431</v>
       </c>
-      <c r="G50" s="6" t="s">
+      <c r="H50" s="6" t="s">
         <v>432</v>
       </c>
-      <c r="H50" s="6" t="s">
+      <c r="I50" s="5" t="s">
         <v>433</v>
       </c>
-      <c r="I50" s="5" t="s">
+      <c r="J50" s="8" t="s">
         <v>434</v>
-      </c>
-      <c r="J50" s="8" t="s">
-        <v>435</v>
       </c>
       <c r="K50" s="9">
         <v>77230</v>
       </c>
       <c r="L50" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A51" s="4">
-        <v>50</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>614</v>
       </c>
       <c r="B51" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="C51" s="6" t="s">
         <v>436</v>
       </c>
-      <c r="C51" s="6" t="s">
+      <c r="D51" s="6" t="s">
         <v>437</v>
       </c>
-      <c r="D51" s="6" t="s">
+      <c r="E51" s="7" t="s">
         <v>438</v>
       </c>
-      <c r="E51" s="7" t="s">
+      <c r="F51" s="6" t="s">
         <v>439</v>
       </c>
-      <c r="F51" s="6" t="s">
+      <c r="G51" s="6" t="s">
         <v>440</v>
       </c>
-      <c r="G51" s="6" t="s">
+      <c r="H51" s="6" t="s">
         <v>441</v>
       </c>
-      <c r="H51" s="6" t="s">
+      <c r="I51" s="5" t="s">
         <v>442</v>
       </c>
-      <c r="I51" s="5" t="s">
+      <c r="J51" s="8" t="s">
         <v>443</v>
-      </c>
-      <c r="J51" s="8" t="s">
-        <v>444</v>
       </c>
       <c r="K51" s="9">
         <v>34712</v>
       </c>
       <c r="L51" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding Test for SignInPage
</commit_message>
<xml_diff>
--- a/data/pet-store-data.xlsx
+++ b/data/pet-store-data.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="765">
   <si>
     <t>ITEM_ID</t>
   </si>
@@ -1862,6 +1862,456 @@
   </si>
   <si>
     <t>b01e31</t>
+  </si>
+  <si>
+    <t>29cc68</t>
+  </si>
+  <si>
+    <t>7acd0e</t>
+  </si>
+  <si>
+    <t>68f07d</t>
+  </si>
+  <si>
+    <t>f54e99</t>
+  </si>
+  <si>
+    <t>5e611c</t>
+  </si>
+  <si>
+    <t>3ff81f</t>
+  </si>
+  <si>
+    <t>f0cf46</t>
+  </si>
+  <si>
+    <t>8f9cc0</t>
+  </si>
+  <si>
+    <t>a78008</t>
+  </si>
+  <si>
+    <t>8fee4f</t>
+  </si>
+  <si>
+    <t>8e1b78</t>
+  </si>
+  <si>
+    <t>c3fd2b</t>
+  </si>
+  <si>
+    <t>270f71</t>
+  </si>
+  <si>
+    <t>148fdd</t>
+  </si>
+  <si>
+    <t>71848d</t>
+  </si>
+  <si>
+    <t>71b1a5</t>
+  </si>
+  <si>
+    <t>a46d0a</t>
+  </si>
+  <si>
+    <t>d1faab</t>
+  </si>
+  <si>
+    <t>fcb298</t>
+  </si>
+  <si>
+    <t>0153a7</t>
+  </si>
+  <si>
+    <t>1a45ce</t>
+  </si>
+  <si>
+    <t>6433d5</t>
+  </si>
+  <si>
+    <t>56195b</t>
+  </si>
+  <si>
+    <t>3b4854</t>
+  </si>
+  <si>
+    <t>aa8244</t>
+  </si>
+  <si>
+    <t>90ed2e</t>
+  </si>
+  <si>
+    <t>178044</t>
+  </si>
+  <si>
+    <t>77771b</t>
+  </si>
+  <si>
+    <t>c2086a</t>
+  </si>
+  <si>
+    <t>1b3672</t>
+  </si>
+  <si>
+    <t>4b3ee7</t>
+  </si>
+  <si>
+    <t>48df61</t>
+  </si>
+  <si>
+    <t>bc680c</t>
+  </si>
+  <si>
+    <t>c7e836</t>
+  </si>
+  <si>
+    <t>e09e2c</t>
+  </si>
+  <si>
+    <t>87e222</t>
+  </si>
+  <si>
+    <t>418971</t>
+  </si>
+  <si>
+    <t>d90eb6</t>
+  </si>
+  <si>
+    <t>9ebcbc</t>
+  </si>
+  <si>
+    <t>5b7357</t>
+  </si>
+  <si>
+    <t>884dc2</t>
+  </si>
+  <si>
+    <t>e66e87</t>
+  </si>
+  <si>
+    <t>09415c</t>
+  </si>
+  <si>
+    <t>d7de3d</t>
+  </si>
+  <si>
+    <t>d28ff1</t>
+  </si>
+  <si>
+    <t>b574ad</t>
+  </si>
+  <si>
+    <t>e7831c</t>
+  </si>
+  <si>
+    <t>165524</t>
+  </si>
+  <si>
+    <t>a32e48</t>
+  </si>
+  <si>
+    <t>42d7b7</t>
+  </si>
+  <si>
+    <t>564de7</t>
+  </si>
+  <si>
+    <t>b60ac4</t>
+  </si>
+  <si>
+    <t>70e4bc</t>
+  </si>
+  <si>
+    <t>157118</t>
+  </si>
+  <si>
+    <t>986af7</t>
+  </si>
+  <si>
+    <t>5d1cef</t>
+  </si>
+  <si>
+    <t>03d8a0</t>
+  </si>
+  <si>
+    <t>87675e</t>
+  </si>
+  <si>
+    <t>b03f75</t>
+  </si>
+  <si>
+    <t>115a06</t>
+  </si>
+  <si>
+    <t>ed6522</t>
+  </si>
+  <si>
+    <t>45f18a</t>
+  </si>
+  <si>
+    <t>85ad28</t>
+  </si>
+  <si>
+    <t>86fdab</t>
+  </si>
+  <si>
+    <t>cc4287</t>
+  </si>
+  <si>
+    <t>0be796</t>
+  </si>
+  <si>
+    <t>709979</t>
+  </si>
+  <si>
+    <t>f300e1</t>
+  </si>
+  <si>
+    <t>5b3761</t>
+  </si>
+  <si>
+    <t>59fb2a</t>
+  </si>
+  <si>
+    <t>b2f292</t>
+  </si>
+  <si>
+    <t>478c13</t>
+  </si>
+  <si>
+    <t>d34d90</t>
+  </si>
+  <si>
+    <t>24b860</t>
+  </si>
+  <si>
+    <t>8d6743</t>
+  </si>
+  <si>
+    <t>49047b</t>
+  </si>
+  <si>
+    <t>e55c31</t>
+  </si>
+  <si>
+    <t>87a9ea</t>
+  </si>
+  <si>
+    <t>79f1bc</t>
+  </si>
+  <si>
+    <t>81cb44</t>
+  </si>
+  <si>
+    <t>92968f</t>
+  </si>
+  <si>
+    <t>3aaa9d</t>
+  </si>
+  <si>
+    <t>9edbe3</t>
+  </si>
+  <si>
+    <t>d926a8</t>
+  </si>
+  <si>
+    <t>abdd83</t>
+  </si>
+  <si>
+    <t>7488dc</t>
+  </si>
+  <si>
+    <t>301e38</t>
+  </si>
+  <si>
+    <t>f0cce4</t>
+  </si>
+  <si>
+    <t>c17b75</t>
+  </si>
+  <si>
+    <t>3733f2</t>
+  </si>
+  <si>
+    <t>d487d0</t>
+  </si>
+  <si>
+    <t>d0c081</t>
+  </si>
+  <si>
+    <t>01a985</t>
+  </si>
+  <si>
+    <t>b85ec2</t>
+  </si>
+  <si>
+    <t>536f29</t>
+  </si>
+  <si>
+    <t>728b92</t>
+  </si>
+  <si>
+    <t>72f550</t>
+  </si>
+  <si>
+    <t>23a509</t>
+  </si>
+  <si>
+    <t>87809c</t>
+  </si>
+  <si>
+    <t>137786</t>
+  </si>
+  <si>
+    <t>1f9af4</t>
+  </si>
+  <si>
+    <t>acfaa9</t>
+  </si>
+  <si>
+    <t>17c9a2</t>
+  </si>
+  <si>
+    <t>0a0b47</t>
+  </si>
+  <si>
+    <t>58e9f6</t>
+  </si>
+  <si>
+    <t>662076</t>
+  </si>
+  <si>
+    <t>e1b204</t>
+  </si>
+  <si>
+    <t>ca2820</t>
+  </si>
+  <si>
+    <t>578915</t>
+  </si>
+  <si>
+    <t>f51925</t>
+  </si>
+  <si>
+    <t>2927c0</t>
+  </si>
+  <si>
+    <t>972589</t>
+  </si>
+  <si>
+    <t>316a91</t>
+  </si>
+  <si>
+    <t>7e8408</t>
+  </si>
+  <si>
+    <t>8fcc8e</t>
+  </si>
+  <si>
+    <t>c919d3</t>
+  </si>
+  <si>
+    <t>6406bc</t>
+  </si>
+  <si>
+    <t>9d7023</t>
+  </si>
+  <si>
+    <t>70be7b</t>
+  </si>
+  <si>
+    <t>f49b4e</t>
+  </si>
+  <si>
+    <t>f1f7e3</t>
+  </si>
+  <si>
+    <t>6e963b</t>
+  </si>
+  <si>
+    <t>38ef05</t>
+  </si>
+  <si>
+    <t>e6c1d1</t>
+  </si>
+  <si>
+    <t>48941e</t>
+  </si>
+  <si>
+    <t>156264</t>
+  </si>
+  <si>
+    <t>637967</t>
+  </si>
+  <si>
+    <t>b0e374</t>
+  </si>
+  <si>
+    <t>d82508</t>
+  </si>
+  <si>
+    <t>e3be1f</t>
+  </si>
+  <si>
+    <t>dbcced</t>
+  </si>
+  <si>
+    <t>73a665</t>
+  </si>
+  <si>
+    <t>65cb3b</t>
+  </si>
+  <si>
+    <t>39351c</t>
+  </si>
+  <si>
+    <t>cf3d7e</t>
+  </si>
+  <si>
+    <t>7ba6ad</t>
+  </si>
+  <si>
+    <t>130a84</t>
+  </si>
+  <si>
+    <t>b5203c</t>
+  </si>
+  <si>
+    <t>e619c1</t>
+  </si>
+  <si>
+    <t>bce836</t>
+  </si>
+  <si>
+    <t>2cfe37</t>
+  </si>
+  <si>
+    <t>f1bf7c</t>
+  </si>
+  <si>
+    <t>6a1040</t>
+  </si>
+  <si>
+    <t>78a860</t>
+  </si>
+  <si>
+    <t>9452ea</t>
+  </si>
+  <si>
+    <t>b84e61</t>
+  </si>
+  <si>
+    <t>74662f</t>
+  </si>
+  <si>
+    <t>0388dc</t>
+  </si>
+  <si>
+    <t>f740fc</t>
+  </si>
+  <si>
+    <t>f7eba0</t>
   </si>
 </sst>
 </file>
@@ -2542,7 +2992,7 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>565</v>
+        <v>715</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>13</v>
@@ -2580,7 +3030,7 @@
     </row>
     <row r="3" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>566</v>
+        <v>716</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>23</v>
@@ -2618,7 +3068,7 @@
     </row>
     <row r="4" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>567</v>
+        <v>717</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>32</v>
@@ -2656,7 +3106,7 @@
     </row>
     <row r="5" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>568</v>
+        <v>718</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>41</v>
@@ -2694,7 +3144,7 @@
     </row>
     <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>569</v>
+        <v>719</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>50</v>
@@ -2732,7 +3182,7 @@
     </row>
     <row r="7" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>570</v>
+        <v>720</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>59</v>
@@ -2770,7 +3220,7 @@
     </row>
     <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>571</v>
+        <v>721</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>68</v>
@@ -2808,7 +3258,7 @@
     </row>
     <row r="9" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>572</v>
+        <v>722</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>77</v>
@@ -2846,7 +3296,7 @@
     </row>
     <row r="10" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>573</v>
+        <v>723</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>86</v>
@@ -2884,7 +3334,7 @@
     </row>
     <row r="11" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>574</v>
+        <v>724</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>95</v>
@@ -2922,7 +3372,7 @@
     </row>
     <row r="12" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>575</v>
+        <v>725</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>104</v>
@@ -2960,7 +3410,7 @@
     </row>
     <row r="13" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>576</v>
+        <v>726</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>113</v>
@@ -2998,7 +3448,7 @@
     </row>
     <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>577</v>
+        <v>727</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>122</v>
@@ -3036,7 +3486,7 @@
     </row>
     <row r="15" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>578</v>
+        <v>728</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>130</v>
@@ -3074,7 +3524,7 @@
     </row>
     <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>579</v>
+        <v>729</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>138</v>
@@ -3112,7 +3562,7 @@
     </row>
     <row r="17" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>580</v>
+        <v>730</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>147</v>
@@ -3150,7 +3600,7 @@
     </row>
     <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>581</v>
+        <v>731</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>155</v>
@@ -3188,7 +3638,7 @@
     </row>
     <row r="19" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>582</v>
+        <v>732</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>164</v>
@@ -3226,7 +3676,7 @@
     </row>
     <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>583</v>
+        <v>733</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>172</v>
@@ -3264,7 +3714,7 @@
     </row>
     <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>584</v>
+        <v>734</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>180</v>
@@ -3302,7 +3752,7 @@
     </row>
     <row r="22" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>585</v>
+        <v>735</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>189</v>
@@ -3340,7 +3790,7 @@
     </row>
     <row r="23" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>586</v>
+        <v>736</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>198</v>
@@ -3378,7 +3828,7 @@
     </row>
     <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>587</v>
+        <v>737</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>206</v>
@@ -3416,7 +3866,7 @@
     </row>
     <row r="25" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
-        <v>588</v>
+        <v>738</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>215</v>
@@ -3454,7 +3904,7 @@
     </row>
     <row r="26" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>589</v>
+        <v>739</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>224</v>
@@ -3492,7 +3942,7 @@
     </row>
     <row r="27" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>590</v>
+        <v>740</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>233</v>
@@ -3530,7 +3980,7 @@
     </row>
     <row r="28" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>591</v>
+        <v>741</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>242</v>
@@ -3568,7 +4018,7 @@
     </row>
     <row r="29" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>592</v>
+        <v>742</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>250</v>
@@ -3606,7 +4056,7 @@
     </row>
     <row r="30" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>593</v>
+        <v>743</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>258</v>
@@ -3644,7 +4094,7 @@
     </row>
     <row r="31" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>594</v>
+        <v>744</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>267</v>
@@ -3682,7 +4132,7 @@
     </row>
     <row r="32" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>595</v>
+        <v>745</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>275</v>
@@ -3720,7 +4170,7 @@
     </row>
     <row r="33" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>596</v>
+        <v>746</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>283</v>
@@ -3758,7 +4208,7 @@
     </row>
     <row r="34" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>597</v>
+        <v>747</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>291</v>
@@ -3796,7 +4246,7 @@
     </row>
     <row r="35" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>598</v>
+        <v>748</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>300</v>
@@ -3834,7 +4284,7 @@
     </row>
     <row r="36" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>599</v>
+        <v>749</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>309</v>
@@ -3872,7 +4322,7 @@
     </row>
     <row r="37" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>600</v>
+        <v>750</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>318</v>
@@ -3910,7 +4360,7 @@
     </row>
     <row r="38" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>601</v>
+        <v>751</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>326</v>
@@ -3948,7 +4398,7 @@
     </row>
     <row r="39" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>602</v>
+        <v>752</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>335</v>
@@ -3986,7 +4436,7 @@
     </row>
     <row r="40" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>603</v>
+        <v>753</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>343</v>
@@ -4024,7 +4474,7 @@
     </row>
     <row r="41" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>604</v>
+        <v>754</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>351</v>
@@ -4062,7 +4512,7 @@
     </row>
     <row r="42" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>605</v>
+        <v>755</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>359</v>
@@ -4100,7 +4550,7 @@
     </row>
     <row r="43" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>606</v>
+        <v>756</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>367</v>
@@ -4138,7 +4588,7 @@
     </row>
     <row r="44" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>607</v>
+        <v>757</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>376</v>
@@ -4176,7 +4626,7 @@
     </row>
     <row r="45" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>608</v>
+        <v>758</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>385</v>
@@ -4214,7 +4664,7 @@
     </row>
     <row r="46" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>609</v>
+        <v>759</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>393</v>
@@ -4252,7 +4702,7 @@
     </row>
     <row r="47" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>610</v>
+        <v>760</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>401</v>
@@ -4290,7 +4740,7 @@
     </row>
     <row r="48" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>611</v>
+        <v>761</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>409</v>
@@ -4328,7 +4778,7 @@
     </row>
     <row r="49" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>612</v>
+        <v>762</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>417</v>
@@ -4366,7 +4816,7 @@
     </row>
     <row r="50" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>613</v>
+        <v>763</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>426</v>
@@ -4404,7 +4854,7 @@
     </row>
     <row r="51" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>614</v>
+        <v>764</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>435</v>

</xml_diff>

<commit_message>
Adding Test for CartPage
</commit_message>
<xml_diff>
--- a/data/pet-store-data.xlsx
+++ b/data/pet-store-data.xlsx
@@ -3,21 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{988A31BE-7465-4334-89A6-CBD04210EBE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{3D353CDE-8154-472A-99A5-7A808A3B96C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="20115" windowHeight="13680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="750" yWindow="750" windowWidth="20145" windowHeight="13680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cart_items" sheetId="1" r:id="rId1"/>
     <sheet name="users" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:H10"/>
+  <oleSize ref="A1:D15"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="765">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="515">
   <si>
     <t>ITEM_ID</t>
   </si>
@@ -1411,757 +1411,7 @@
     <t>https://petstore.octoperf.com/actions/Catalog.action?viewItem=&amp;itemId=EST-13</t>
   </si>
   <si>
-    <t>61c28</t>
-  </si>
-  <si>
-    <t>33aea</t>
-  </si>
-  <si>
-    <t>1dfdc</t>
-  </si>
-  <si>
-    <t>0981e</t>
-  </si>
-  <si>
-    <t>7304d</t>
-  </si>
-  <si>
-    <t>2c116</t>
-  </si>
-  <si>
-    <t>dd3c1</t>
-  </si>
-  <si>
-    <t>9abfa</t>
-  </si>
-  <si>
-    <t>e2447</t>
-  </si>
-  <si>
-    <t>b1b73</t>
-  </si>
-  <si>
-    <t>ab663</t>
-  </si>
-  <si>
-    <t>b350d</t>
-  </si>
-  <si>
-    <t>1dd90</t>
-  </si>
-  <si>
-    <t>cb275</t>
-  </si>
-  <si>
-    <t>613e0</t>
-  </si>
-  <si>
-    <t>93cff</t>
-  </si>
-  <si>
-    <t>af10d</t>
-  </si>
-  <si>
-    <t>97191</t>
-  </si>
-  <si>
-    <t>0b93b</t>
-  </si>
-  <si>
-    <t>41613</t>
-  </si>
-  <si>
-    <t>4e3e5</t>
-  </si>
-  <si>
-    <t>68995</t>
-  </si>
-  <si>
-    <t>23517</t>
-  </si>
-  <si>
-    <t>e8136</t>
-  </si>
-  <si>
-    <t>0ed1c</t>
-  </si>
-  <si>
-    <t>ae2e5</t>
-  </si>
-  <si>
-    <t>e93bc</t>
-  </si>
-  <si>
-    <t>ae27c</t>
-  </si>
-  <si>
-    <t>22e19</t>
-  </si>
-  <si>
-    <t>264a5</t>
-  </si>
-  <si>
-    <t>c11f8</t>
-  </si>
-  <si>
-    <t>54439</t>
-  </si>
-  <si>
-    <t>75fa3</t>
-  </si>
-  <si>
-    <t>21875</t>
-  </si>
-  <si>
-    <t>853a3</t>
-  </si>
-  <si>
-    <t>b02ea</t>
-  </si>
-  <si>
-    <t>2f578</t>
-  </si>
-  <si>
-    <t>8229d</t>
-  </si>
-  <si>
-    <t>81996</t>
-  </si>
-  <si>
-    <t>5ce18</t>
-  </si>
-  <si>
-    <t>37c73</t>
-  </si>
-  <si>
-    <t>c238b</t>
-  </si>
-  <si>
-    <t>722df</t>
-  </si>
-  <si>
-    <t>c85f0</t>
-  </si>
-  <si>
-    <t>33051</t>
-  </si>
-  <si>
-    <t>0fae5</t>
-  </si>
-  <si>
-    <t>838cf</t>
-  </si>
-  <si>
-    <t>0df35</t>
-  </si>
-  <si>
-    <t>2d8e9</t>
-  </si>
-  <si>
-    <t>ed274</t>
-  </si>
-  <si>
     <t>ID</t>
-  </si>
-  <si>
-    <t>b74d29</t>
-  </si>
-  <si>
-    <t>abe1d2</t>
-  </si>
-  <si>
-    <t>ec328b</t>
-  </si>
-  <si>
-    <t>eb6c35</t>
-  </si>
-  <si>
-    <t>fd35f6</t>
-  </si>
-  <si>
-    <t>85a259</t>
-  </si>
-  <si>
-    <t>e7139e</t>
-  </si>
-  <si>
-    <t>a9d7f1</t>
-  </si>
-  <si>
-    <t>3d03d2</t>
-  </si>
-  <si>
-    <t>338519</t>
-  </si>
-  <si>
-    <t>9088eb</t>
-  </si>
-  <si>
-    <t>97ad86</t>
-  </si>
-  <si>
-    <t>b59715</t>
-  </si>
-  <si>
-    <t>5e8aeb</t>
-  </si>
-  <si>
-    <t>b6cc38</t>
-  </si>
-  <si>
-    <t>94e901</t>
-  </si>
-  <si>
-    <t>19fe01</t>
-  </si>
-  <si>
-    <t>b3fe19</t>
-  </si>
-  <si>
-    <t>d7d23a</t>
-  </si>
-  <si>
-    <t>879555</t>
-  </si>
-  <si>
-    <t>baa53a</t>
-  </si>
-  <si>
-    <t>4eb770</t>
-  </si>
-  <si>
-    <t>2dccc8</t>
-  </si>
-  <si>
-    <t>eda27a</t>
-  </si>
-  <si>
-    <t>a79e28</t>
-  </si>
-  <si>
-    <t>051aaf</t>
-  </si>
-  <si>
-    <t>f3e00c</t>
-  </si>
-  <si>
-    <t>daa81f</t>
-  </si>
-  <si>
-    <t>6bf61c</t>
-  </si>
-  <si>
-    <t>2d7ea7</t>
-  </si>
-  <si>
-    <t>e28783</t>
-  </si>
-  <si>
-    <t>275854</t>
-  </si>
-  <si>
-    <t>89f656</t>
-  </si>
-  <si>
-    <t>575962</t>
-  </si>
-  <si>
-    <t>63990a</t>
-  </si>
-  <si>
-    <t>a53584</t>
-  </si>
-  <si>
-    <t>5649fb</t>
-  </si>
-  <si>
-    <t>53077f</t>
-  </si>
-  <si>
-    <t>e4dbc8</t>
-  </si>
-  <si>
-    <t>57b0c1</t>
-  </si>
-  <si>
-    <t>8f4467</t>
-  </si>
-  <si>
-    <t>c5503e</t>
-  </si>
-  <si>
-    <t>60548b</t>
-  </si>
-  <si>
-    <t>09cb8b</t>
-  </si>
-  <si>
-    <t>eb3085</t>
-  </si>
-  <si>
-    <t>77bbc3</t>
-  </si>
-  <si>
-    <t>f59058</t>
-  </si>
-  <si>
-    <t>6ebf47</t>
-  </si>
-  <si>
-    <t>d88619</t>
-  </si>
-  <si>
-    <t>d44a83</t>
-  </si>
-  <si>
-    <t>56b62f</t>
-  </si>
-  <si>
-    <t>d51c34</t>
-  </si>
-  <si>
-    <t>b0c995</t>
-  </si>
-  <si>
-    <t>838d29</t>
-  </si>
-  <si>
-    <t>e599db</t>
-  </si>
-  <si>
-    <t>b227d8</t>
-  </si>
-  <si>
-    <t>7fb0f4</t>
-  </si>
-  <si>
-    <t>087e9d</t>
-  </si>
-  <si>
-    <t>945fdd</t>
-  </si>
-  <si>
-    <t>622948</t>
-  </si>
-  <si>
-    <t>7e7b41</t>
-  </si>
-  <si>
-    <t>482fb9</t>
-  </si>
-  <si>
-    <t>b601cc</t>
-  </si>
-  <si>
-    <t>b4292a</t>
-  </si>
-  <si>
-    <t>c8a1fa</t>
-  </si>
-  <si>
-    <t>85ff05</t>
-  </si>
-  <si>
-    <t>92243f</t>
-  </si>
-  <si>
-    <t>34258f</t>
-  </si>
-  <si>
-    <t>1aec88</t>
-  </si>
-  <si>
-    <t>c68e82</t>
-  </si>
-  <si>
-    <t>28889d</t>
-  </si>
-  <si>
-    <t>ef412a</t>
-  </si>
-  <si>
-    <t>c7abd6</t>
-  </si>
-  <si>
-    <t>d8011c</t>
-  </si>
-  <si>
-    <t>4cf789</t>
-  </si>
-  <si>
-    <t>f009a3</t>
-  </si>
-  <si>
-    <t>516c03</t>
-  </si>
-  <si>
-    <t>407e8c</t>
-  </si>
-  <si>
-    <t>99b08f</t>
-  </si>
-  <si>
-    <t>02237b</t>
-  </si>
-  <si>
-    <t>09b5dc</t>
-  </si>
-  <si>
-    <t>594516</t>
-  </si>
-  <si>
-    <t>68528c</t>
-  </si>
-  <si>
-    <t>16ffc8</t>
-  </si>
-  <si>
-    <t>4159f2</t>
-  </si>
-  <si>
-    <t>c74fa5</t>
-  </si>
-  <si>
-    <t>a3e086</t>
-  </si>
-  <si>
-    <t>a6615e</t>
-  </si>
-  <si>
-    <t>a36d3e</t>
-  </si>
-  <si>
-    <t>03554d</t>
-  </si>
-  <si>
-    <t>cec4e1</t>
-  </si>
-  <si>
-    <t>f00e8a</t>
-  </si>
-  <si>
-    <t>41ea64</t>
-  </si>
-  <si>
-    <t>118246</t>
-  </si>
-  <si>
-    <t>fadd3d</t>
-  </si>
-  <si>
-    <t>0705c8</t>
-  </si>
-  <si>
-    <t>4d19f4</t>
-  </si>
-  <si>
-    <t>2ce623</t>
-  </si>
-  <si>
-    <t>211f57</t>
-  </si>
-  <si>
-    <t>b01e31</t>
-  </si>
-  <si>
-    <t>29cc68</t>
-  </si>
-  <si>
-    <t>7acd0e</t>
-  </si>
-  <si>
-    <t>68f07d</t>
-  </si>
-  <si>
-    <t>f54e99</t>
-  </si>
-  <si>
-    <t>5e611c</t>
-  </si>
-  <si>
-    <t>3ff81f</t>
-  </si>
-  <si>
-    <t>f0cf46</t>
-  </si>
-  <si>
-    <t>8f9cc0</t>
-  </si>
-  <si>
-    <t>a78008</t>
-  </si>
-  <si>
-    <t>8fee4f</t>
-  </si>
-  <si>
-    <t>8e1b78</t>
-  </si>
-  <si>
-    <t>c3fd2b</t>
-  </si>
-  <si>
-    <t>270f71</t>
-  </si>
-  <si>
-    <t>148fdd</t>
-  </si>
-  <si>
-    <t>71848d</t>
-  </si>
-  <si>
-    <t>71b1a5</t>
-  </si>
-  <si>
-    <t>a46d0a</t>
-  </si>
-  <si>
-    <t>d1faab</t>
-  </si>
-  <si>
-    <t>fcb298</t>
-  </si>
-  <si>
-    <t>0153a7</t>
-  </si>
-  <si>
-    <t>1a45ce</t>
-  </si>
-  <si>
-    <t>6433d5</t>
-  </si>
-  <si>
-    <t>56195b</t>
-  </si>
-  <si>
-    <t>3b4854</t>
-  </si>
-  <si>
-    <t>aa8244</t>
-  </si>
-  <si>
-    <t>90ed2e</t>
-  </si>
-  <si>
-    <t>178044</t>
-  </si>
-  <si>
-    <t>77771b</t>
-  </si>
-  <si>
-    <t>c2086a</t>
-  </si>
-  <si>
-    <t>1b3672</t>
-  </si>
-  <si>
-    <t>4b3ee7</t>
-  </si>
-  <si>
-    <t>48df61</t>
-  </si>
-  <si>
-    <t>bc680c</t>
-  </si>
-  <si>
-    <t>c7e836</t>
-  </si>
-  <si>
-    <t>e09e2c</t>
-  </si>
-  <si>
-    <t>87e222</t>
-  </si>
-  <si>
-    <t>418971</t>
-  </si>
-  <si>
-    <t>d90eb6</t>
-  </si>
-  <si>
-    <t>9ebcbc</t>
-  </si>
-  <si>
-    <t>5b7357</t>
-  </si>
-  <si>
-    <t>884dc2</t>
-  </si>
-  <si>
-    <t>e66e87</t>
-  </si>
-  <si>
-    <t>09415c</t>
-  </si>
-  <si>
-    <t>d7de3d</t>
-  </si>
-  <si>
-    <t>d28ff1</t>
-  </si>
-  <si>
-    <t>b574ad</t>
-  </si>
-  <si>
-    <t>e7831c</t>
-  </si>
-  <si>
-    <t>165524</t>
-  </si>
-  <si>
-    <t>a32e48</t>
-  </si>
-  <si>
-    <t>42d7b7</t>
-  </si>
-  <si>
-    <t>564de7</t>
-  </si>
-  <si>
-    <t>b60ac4</t>
-  </si>
-  <si>
-    <t>70e4bc</t>
-  </si>
-  <si>
-    <t>157118</t>
-  </si>
-  <si>
-    <t>986af7</t>
-  </si>
-  <si>
-    <t>5d1cef</t>
-  </si>
-  <si>
-    <t>03d8a0</t>
-  </si>
-  <si>
-    <t>87675e</t>
-  </si>
-  <si>
-    <t>b03f75</t>
-  </si>
-  <si>
-    <t>115a06</t>
-  </si>
-  <si>
-    <t>ed6522</t>
-  </si>
-  <si>
-    <t>45f18a</t>
-  </si>
-  <si>
-    <t>85ad28</t>
-  </si>
-  <si>
-    <t>86fdab</t>
-  </si>
-  <si>
-    <t>cc4287</t>
-  </si>
-  <si>
-    <t>0be796</t>
-  </si>
-  <si>
-    <t>709979</t>
-  </si>
-  <si>
-    <t>f300e1</t>
-  </si>
-  <si>
-    <t>5b3761</t>
-  </si>
-  <si>
-    <t>59fb2a</t>
-  </si>
-  <si>
-    <t>b2f292</t>
-  </si>
-  <si>
-    <t>478c13</t>
-  </si>
-  <si>
-    <t>d34d90</t>
-  </si>
-  <si>
-    <t>24b860</t>
-  </si>
-  <si>
-    <t>8d6743</t>
-  </si>
-  <si>
-    <t>49047b</t>
-  </si>
-  <si>
-    <t>e55c31</t>
-  </si>
-  <si>
-    <t>87a9ea</t>
-  </si>
-  <si>
-    <t>79f1bc</t>
-  </si>
-  <si>
-    <t>81cb44</t>
-  </si>
-  <si>
-    <t>92968f</t>
-  </si>
-  <si>
-    <t>3aaa9d</t>
-  </si>
-  <si>
-    <t>9edbe3</t>
-  </si>
-  <si>
-    <t>d926a8</t>
-  </si>
-  <si>
-    <t>abdd83</t>
-  </si>
-  <si>
-    <t>7488dc</t>
-  </si>
-  <si>
-    <t>301e38</t>
-  </si>
-  <si>
-    <t>f0cce4</t>
-  </si>
-  <si>
-    <t>c17b75</t>
-  </si>
-  <si>
-    <t>3733f2</t>
-  </si>
-  <si>
-    <t>d487d0</t>
-  </si>
-  <si>
-    <t>d0c081</t>
-  </si>
-  <si>
-    <t>01a985</t>
-  </si>
-  <si>
-    <t>b85ec2</t>
-  </si>
-  <si>
-    <t>536f29</t>
-  </si>
-  <si>
-    <t>728b92</t>
-  </si>
-  <si>
-    <t>72f550</t>
-  </si>
-  <si>
-    <t>23a509</t>
-  </si>
-  <si>
-    <t>87809c</t>
-  </si>
-  <si>
-    <t>137786</t>
   </si>
   <si>
     <t>1f9af4</t>
@@ -2318,7 +1568,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2820,14 +2069,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="28.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="108.0" collapsed="true"/>
+    <col min="1" max="1" width="28.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="108" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -2939,22 +2188,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" style="3" width="17.28515625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="3" width="25.85546875" collapsed="true"/>
-    <col min="6" max="6" style="3" width="17.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="3" width="27.42578125" collapsed="true"/>
-    <col min="8" max="16384" style="3" width="17.28515625" collapsed="true"/>
+    <col min="1" max="4" width="17.28515625" style="3" collapsed="1"/>
+    <col min="5" max="5" width="25.85546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.28515625" style="3" collapsed="1"/>
+    <col min="7" max="7" width="27.42578125" style="3" customWidth="1" collapsed="1"/>
+    <col min="8" max="16384" width="17.28515625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>514</v>
+        <v>464</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
@@ -2992,7 +2241,7 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>715</v>
+        <v>465</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>13</v>
@@ -3030,7 +2279,7 @@
     </row>
     <row r="3" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>716</v>
+        <v>466</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>23</v>
@@ -3068,7 +2317,7 @@
     </row>
     <row r="4" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>717</v>
+        <v>467</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>32</v>
@@ -3106,7 +2355,7 @@
     </row>
     <row r="5" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>718</v>
+        <v>468</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>41</v>
@@ -3144,7 +2393,7 @@
     </row>
     <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>719</v>
+        <v>469</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>50</v>
@@ -3182,7 +2431,7 @@
     </row>
     <row r="7" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>720</v>
+        <v>470</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>59</v>
@@ -3220,7 +2469,7 @@
     </row>
     <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>721</v>
+        <v>471</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>68</v>
@@ -3258,7 +2507,7 @@
     </row>
     <row r="9" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>722</v>
+        <v>472</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>77</v>
@@ -3296,7 +2545,7 @@
     </row>
     <row r="10" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>723</v>
+        <v>473</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>86</v>
@@ -3334,7 +2583,7 @@
     </row>
     <row r="11" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>724</v>
+        <v>474</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>95</v>
@@ -3372,7 +2621,7 @@
     </row>
     <row r="12" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>725</v>
+        <v>475</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>104</v>
@@ -3410,7 +2659,7 @@
     </row>
     <row r="13" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>726</v>
+        <v>476</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>113</v>
@@ -3448,7 +2697,7 @@
     </row>
     <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>727</v>
+        <v>477</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>122</v>
@@ -3486,7 +2735,7 @@
     </row>
     <row r="15" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>728</v>
+        <v>478</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>130</v>
@@ -3524,7 +2773,7 @@
     </row>
     <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>729</v>
+        <v>479</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>138</v>
@@ -3562,7 +2811,7 @@
     </row>
     <row r="17" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>730</v>
+        <v>480</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>147</v>
@@ -3600,7 +2849,7 @@
     </row>
     <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>731</v>
+        <v>481</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>155</v>
@@ -3638,7 +2887,7 @@
     </row>
     <row r="19" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>732</v>
+        <v>482</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>164</v>
@@ -3676,7 +2925,7 @@
     </row>
     <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>733</v>
+        <v>483</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>172</v>
@@ -3714,7 +2963,7 @@
     </row>
     <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>734</v>
+        <v>484</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>180</v>
@@ -3752,7 +3001,7 @@
     </row>
     <row r="22" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>735</v>
+        <v>485</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>189</v>
@@ -3790,7 +3039,7 @@
     </row>
     <row r="23" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>736</v>
+        <v>486</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>198</v>
@@ -3828,7 +3077,7 @@
     </row>
     <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>737</v>
+        <v>487</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>206</v>
@@ -3866,7 +3115,7 @@
     </row>
     <row r="25" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
-        <v>738</v>
+        <v>488</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>215</v>
@@ -3904,7 +3153,7 @@
     </row>
     <row r="26" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>739</v>
+        <v>489</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>224</v>
@@ -3942,7 +3191,7 @@
     </row>
     <row r="27" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>740</v>
+        <v>490</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>233</v>
@@ -3980,7 +3229,7 @@
     </row>
     <row r="28" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>741</v>
+        <v>491</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>242</v>
@@ -4018,7 +3267,7 @@
     </row>
     <row r="29" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>742</v>
+        <v>492</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>250</v>
@@ -4056,7 +3305,7 @@
     </row>
     <row r="30" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>743</v>
+        <v>493</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>258</v>
@@ -4094,7 +3343,7 @@
     </row>
     <row r="31" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>744</v>
+        <v>494</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>267</v>
@@ -4132,7 +3381,7 @@
     </row>
     <row r="32" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>745</v>
+        <v>495</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>275</v>
@@ -4170,7 +3419,7 @@
     </row>
     <row r="33" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>746</v>
+        <v>496</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>283</v>
@@ -4208,7 +3457,7 @@
     </row>
     <row r="34" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>747</v>
+        <v>497</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>291</v>
@@ -4246,7 +3495,7 @@
     </row>
     <row r="35" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>748</v>
+        <v>498</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>300</v>
@@ -4284,7 +3533,7 @@
     </row>
     <row r="36" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>749</v>
+        <v>499</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>309</v>
@@ -4322,7 +3571,7 @@
     </row>
     <row r="37" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>750</v>
+        <v>500</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>318</v>
@@ -4360,7 +3609,7 @@
     </row>
     <row r="38" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>751</v>
+        <v>501</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>326</v>
@@ -4398,7 +3647,7 @@
     </row>
     <row r="39" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>752</v>
+        <v>502</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>335</v>
@@ -4436,7 +3685,7 @@
     </row>
     <row r="40" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>753</v>
+        <v>503</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>343</v>
@@ -4474,7 +3723,7 @@
     </row>
     <row r="41" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>754</v>
+        <v>504</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>351</v>
@@ -4512,7 +3761,7 @@
     </row>
     <row r="42" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>755</v>
+        <v>505</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>359</v>
@@ -4550,7 +3799,7 @@
     </row>
     <row r="43" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>756</v>
+        <v>506</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>367</v>
@@ -4588,7 +3837,7 @@
     </row>
     <row r="44" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>757</v>
+        <v>507</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>376</v>
@@ -4626,7 +3875,7 @@
     </row>
     <row r="45" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>758</v>
+        <v>508</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>385</v>
@@ -4664,7 +3913,7 @@
     </row>
     <row r="46" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>759</v>
+        <v>509</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>393</v>
@@ -4702,7 +3951,7 @@
     </row>
     <row r="47" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>760</v>
+        <v>510</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>401</v>
@@ -4740,7 +3989,7 @@
     </row>
     <row r="48" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>761</v>
+        <v>511</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>409</v>
@@ -4778,7 +4027,7 @@
     </row>
     <row r="49" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>762</v>
+        <v>512</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>417</v>
@@ -4816,7 +4065,7 @@
     </row>
     <row r="50" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>763</v>
+        <v>513</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>426</v>
@@ -4854,7 +4103,7 @@
     </row>
     <row r="51" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>764</v>
+        <v>514</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>435</v>

</xml_diff>

<commit_message>
Edited some tests and pages
</commit_message>
<xml_diff>
--- a/data/pet-store-data.xlsx
+++ b/data/pet-store-data.xlsx
@@ -3,21 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{3D353CDE-8154-472A-99A5-7A808A3B96C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{E87251E8-1F50-4BB7-8C9C-EF04FE59AA46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="750" yWindow="750" windowWidth="20145" windowHeight="13680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="20175" windowHeight="13800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cart_items" sheetId="1" r:id="rId1"/>
     <sheet name="users" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:D15"/>
+  <oleSize ref="A1:F10"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="574">
   <si>
     <t>ITEM_ID</t>
   </si>
@@ -1562,12 +1562,190 @@
   </si>
   <si>
     <t>f7eba0</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>afcd9c</t>
+  </si>
+  <si>
+    <t>e36919</t>
+  </si>
+  <si>
+    <t>c840df</t>
+  </si>
+  <si>
+    <t>98f904</t>
+  </si>
+  <si>
+    <t>06e75c</t>
+  </si>
+  <si>
+    <t>42aebd</t>
+  </si>
+  <si>
+    <t>fc62a6</t>
+  </si>
+  <si>
+    <t>d03d73</t>
+  </si>
+  <si>
+    <t>71ab6d</t>
+  </si>
+  <si>
+    <t>381a31</t>
+  </si>
+  <si>
+    <t>c0eae2</t>
+  </si>
+  <si>
+    <t>f530d5</t>
+  </si>
+  <si>
+    <t>740262</t>
+  </si>
+  <si>
+    <t>061dc5</t>
+  </si>
+  <si>
+    <t>eb3d80</t>
+  </si>
+  <si>
+    <t>4ea324</t>
+  </si>
+  <si>
+    <t>86e15f</t>
+  </si>
+  <si>
+    <t>135b42</t>
+  </si>
+  <si>
+    <t>36338e</t>
+  </si>
+  <si>
+    <t>d5941f</t>
+  </si>
+  <si>
+    <t>fb2547</t>
+  </si>
+  <si>
+    <t>0db4d6</t>
+  </si>
+  <si>
+    <t>5d28d7</t>
+  </si>
+  <si>
+    <t>446b7f</t>
+  </si>
+  <si>
+    <t>9bf71c</t>
+  </si>
+  <si>
+    <t>965e38</t>
+  </si>
+  <si>
+    <t>fad363</t>
+  </si>
+  <si>
+    <t>95f8bf</t>
+  </si>
+  <si>
+    <t>d6594f</t>
+  </si>
+  <si>
+    <t>d8b649</t>
+  </si>
+  <si>
+    <t>2ec4a6</t>
+  </si>
+  <si>
+    <t>9e1237</t>
+  </si>
+  <si>
+    <t>f405cb</t>
+  </si>
+  <si>
+    <t>b00734</t>
+  </si>
+  <si>
+    <t>35086b</t>
+  </si>
+  <si>
+    <t>78d579</t>
+  </si>
+  <si>
+    <t>10fdd4</t>
+  </si>
+  <si>
+    <t>6fb309</t>
+  </si>
+  <si>
+    <t>d230e8</t>
+  </si>
+  <si>
+    <t>a6df31</t>
+  </si>
+  <si>
+    <t>c82c57</t>
+  </si>
+  <si>
+    <t>0c2456</t>
+  </si>
+  <si>
+    <t>287464</t>
+  </si>
+  <si>
+    <t>7454d0</t>
+  </si>
+  <si>
+    <t>ba0b71</t>
+  </si>
+  <si>
+    <t>be9acc</t>
+  </si>
+  <si>
+    <t>87ef03</t>
+  </si>
+  <si>
+    <t>91ad49</t>
+  </si>
+  <si>
+    <t>bfab06</t>
+  </si>
+  <si>
+    <t>cfb4e5</t>
+  </si>
+  <si>
+    <t>english</t>
+  </si>
+  <si>
+    <t>japanese</t>
+  </si>
+  <si>
+    <t>FISH</t>
+  </si>
+  <si>
+    <t>CATS</t>
+  </si>
+  <si>
+    <t>BIRDS</t>
+  </si>
+  <si>
+    <t>REPTILES</t>
+  </si>
+  <si>
+    <t>DOGS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2069,14 +2247,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="108" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="28.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="108.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -2186,22 +2364,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L51"/>
+  <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="17.28515625" style="3" collapsed="1"/>
-    <col min="5" max="5" width="25.85546875" style="3" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.28515625" style="3" collapsed="1"/>
-    <col min="7" max="7" width="27.42578125" style="3" customWidth="1" collapsed="1"/>
-    <col min="8" max="16384" width="17.28515625" style="3" collapsed="1"/>
+    <col min="1" max="4" style="3" width="17.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="3" width="25.85546875" collapsed="true"/>
+    <col min="6" max="6" style="3" width="17.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="3" width="27.42578125" collapsed="true"/>
+    <col min="8" max="16384" style="3" width="17.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>464</v>
       </c>
@@ -2238,10 +2416,16 @@
       <c r="L1" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M1" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>465</v>
+        <v>517</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>13</v>
@@ -2276,10 +2460,16 @@
       <c r="L2" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M2" t="s">
+        <v>567</v>
+      </c>
+      <c r="N2" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>466</v>
+        <v>518</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>23</v>
@@ -2314,10 +2504,16 @@
       <c r="L3" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M3" t="s">
+        <v>567</v>
+      </c>
+      <c r="N3" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>467</v>
+        <v>519</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>32</v>
@@ -2352,10 +2548,16 @@
       <c r="L4" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M4" t="s">
+        <v>568</v>
+      </c>
+      <c r="N4" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>468</v>
+        <v>520</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>41</v>
@@ -2390,10 +2592,16 @@
       <c r="L5" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M5" t="s">
+        <v>567</v>
+      </c>
+      <c r="N5" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>469</v>
+        <v>521</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>50</v>
@@ -2428,10 +2636,16 @@
       <c r="L6" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M6" t="s">
+        <v>568</v>
+      </c>
+      <c r="N6" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>470</v>
+        <v>522</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>59</v>
@@ -2466,10 +2680,16 @@
       <c r="L7" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M7" t="s">
+        <v>567</v>
+      </c>
+      <c r="N7" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>471</v>
+        <v>523</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>68</v>
@@ -2504,10 +2724,16 @@
       <c r="L8" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M8" t="s">
+        <v>568</v>
+      </c>
+      <c r="N8" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>472</v>
+        <v>524</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>77</v>
@@ -2542,10 +2768,16 @@
       <c r="L9" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M9" t="s">
+        <v>568</v>
+      </c>
+      <c r="N9" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>473</v>
+        <v>525</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>86</v>
@@ -2580,10 +2812,16 @@
       <c r="L10" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M10" t="s">
+        <v>568</v>
+      </c>
+      <c r="N10" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>474</v>
+        <v>526</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>95</v>
@@ -2618,10 +2856,16 @@
       <c r="L11" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M11" t="s">
+        <v>567</v>
+      </c>
+      <c r="N11" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>475</v>
+        <v>527</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>104</v>
@@ -2656,10 +2900,16 @@
       <c r="L12" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M12" t="s">
+        <v>567</v>
+      </c>
+      <c r="N12" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>476</v>
+        <v>528</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>113</v>
@@ -2694,10 +2944,16 @@
       <c r="L13" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M13" t="s">
+        <v>567</v>
+      </c>
+      <c r="N13" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>477</v>
+        <v>529</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>122</v>
@@ -2732,10 +2988,16 @@
       <c r="L14" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M14" t="s">
+        <v>568</v>
+      </c>
+      <c r="N14" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>478</v>
+        <v>530</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>130</v>
@@ -2770,10 +3032,16 @@
       <c r="L15" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M15" t="s">
+        <v>567</v>
+      </c>
+      <c r="N15" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>479</v>
+        <v>531</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>138</v>
@@ -2808,10 +3076,16 @@
       <c r="L16" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="M16" t="s">
+        <v>568</v>
+      </c>
+      <c r="N16" t="s">
+        <v>569</v>
+      </c>
     </row>
     <row r="17" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>480</v>
+        <v>532</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>147</v>
@@ -2846,10 +3120,16 @@
       <c r="L17" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="M17" t="s">
+        <v>567</v>
+      </c>
+      <c r="N17" t="s">
+        <v>571</v>
+      </c>
     </row>
     <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>481</v>
+        <v>533</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>155</v>
@@ -2884,10 +3164,16 @@
       <c r="L18" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="M18" t="s">
+        <v>568</v>
+      </c>
+      <c r="N18" t="s">
+        <v>573</v>
+      </c>
     </row>
     <row r="19" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>482</v>
+        <v>534</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>164</v>
@@ -2922,10 +3208,16 @@
       <c r="L19" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="M19" t="s">
+        <v>568</v>
+      </c>
+      <c r="N19" t="s">
+        <v>570</v>
+      </c>
     </row>
     <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>483</v>
+        <v>535</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>172</v>
@@ -2960,10 +3252,16 @@
       <c r="L20" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="M20" t="s">
+        <v>567</v>
+      </c>
+      <c r="N20" t="s">
+        <v>572</v>
+      </c>
     </row>
     <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>484</v>
+        <v>536</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>180</v>
@@ -2998,10 +3296,16 @@
       <c r="L21" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="M21" t="s">
+        <v>568</v>
+      </c>
+      <c r="N21" t="s">
+        <v>572</v>
+      </c>
     </row>
     <row r="22" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>485</v>
+        <v>537</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>189</v>
@@ -3036,10 +3340,16 @@
       <c r="L22" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="M22" t="s">
+        <v>568</v>
+      </c>
+      <c r="N22" t="s">
+        <v>570</v>
+      </c>
     </row>
     <row r="23" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>486</v>
+        <v>538</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>198</v>
@@ -3074,10 +3384,16 @@
       <c r="L23" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="M23" t="s">
+        <v>568</v>
+      </c>
+      <c r="N23" t="s">
+        <v>573</v>
+      </c>
     </row>
     <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>487</v>
+        <v>539</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>206</v>
@@ -3112,10 +3428,16 @@
       <c r="L24" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="M24" t="s">
+        <v>568</v>
+      </c>
+      <c r="N24" t="s">
+        <v>571</v>
+      </c>
     </row>
     <row r="25" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
-        <v>488</v>
+        <v>540</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>215</v>
@@ -3150,10 +3472,16 @@
       <c r="L25" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="M25" t="s">
+        <v>567</v>
+      </c>
+      <c r="N25" t="s">
+        <v>573</v>
+      </c>
     </row>
     <row r="26" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>489</v>
+        <v>541</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>224</v>
@@ -3188,10 +3516,16 @@
       <c r="L26" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="M26" t="s">
+        <v>567</v>
+      </c>
+      <c r="N26" t="s">
+        <v>571</v>
+      </c>
     </row>
     <row r="27" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>490</v>
+        <v>542</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>233</v>
@@ -3226,10 +3560,16 @@
       <c r="L27" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="M27" t="s">
+        <v>567</v>
+      </c>
+      <c r="N27" t="s">
+        <v>573</v>
+      </c>
     </row>
     <row r="28" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>491</v>
+        <v>543</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>242</v>
@@ -3264,10 +3604,16 @@
       <c r="L28" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="M28" t="s">
+        <v>568</v>
+      </c>
+      <c r="N28" t="s">
+        <v>570</v>
+      </c>
     </row>
     <row r="29" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>492</v>
+        <v>544</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>250</v>
@@ -3302,10 +3648,16 @@
       <c r="L29" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="M29" t="s">
+        <v>568</v>
+      </c>
+      <c r="N29" t="s">
+        <v>569</v>
+      </c>
     </row>
     <row r="30" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>493</v>
+        <v>545</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>258</v>
@@ -3340,10 +3692,16 @@
       <c r="L30" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="M30" t="s">
+        <v>567</v>
+      </c>
+      <c r="N30" t="s">
+        <v>572</v>
+      </c>
     </row>
     <row r="31" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>494</v>
+        <v>546</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>267</v>
@@ -3378,10 +3736,16 @@
       <c r="L31" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="M31" t="s">
+        <v>568</v>
+      </c>
+      <c r="N31" t="s">
+        <v>571</v>
+      </c>
     </row>
     <row r="32" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>495</v>
+        <v>547</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>275</v>
@@ -3416,10 +3780,16 @@
       <c r="L32" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="M32" t="s">
+        <v>568</v>
+      </c>
+      <c r="N32" t="s">
+        <v>571</v>
+      </c>
     </row>
     <row r="33" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>496</v>
+        <v>548</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>283</v>
@@ -3454,10 +3824,16 @@
       <c r="L33" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="M33" t="s">
+        <v>567</v>
+      </c>
+      <c r="N33" t="s">
+        <v>569</v>
+      </c>
     </row>
     <row r="34" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>497</v>
+        <v>549</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>291</v>
@@ -3492,10 +3868,16 @@
       <c r="L34" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="M34" t="s">
+        <v>568</v>
+      </c>
+      <c r="N34" t="s">
+        <v>573</v>
+      </c>
     </row>
     <row r="35" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>498</v>
+        <v>550</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>300</v>
@@ -3530,10 +3912,16 @@
       <c r="L35" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="M35" t="s">
+        <v>568</v>
+      </c>
+      <c r="N35" t="s">
+        <v>569</v>
+      </c>
     </row>
     <row r="36" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>499</v>
+        <v>551</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>309</v>
@@ -3568,10 +3956,16 @@
       <c r="L36" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="M36" t="s">
+        <v>568</v>
+      </c>
+      <c r="N36" t="s">
+        <v>571</v>
+      </c>
     </row>
     <row r="37" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>500</v>
+        <v>552</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>318</v>
@@ -3606,10 +4000,16 @@
       <c r="L37" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="M37" t="s">
+        <v>567</v>
+      </c>
+      <c r="N37" t="s">
+        <v>569</v>
+      </c>
     </row>
     <row r="38" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>501</v>
+        <v>553</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>326</v>
@@ -3644,10 +4044,16 @@
       <c r="L38" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="M38" t="s">
+        <v>568</v>
+      </c>
+      <c r="N38" t="s">
+        <v>572</v>
+      </c>
     </row>
     <row r="39" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>502</v>
+        <v>554</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>335</v>
@@ -3682,10 +4088,16 @@
       <c r="L39" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="M39" t="s">
+        <v>567</v>
+      </c>
+      <c r="N39" t="s">
+        <v>572</v>
+      </c>
     </row>
     <row r="40" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>503</v>
+        <v>555</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>343</v>
@@ -3720,10 +4132,16 @@
       <c r="L40" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="M40" t="s">
+        <v>567</v>
+      </c>
+      <c r="N40" t="s">
+        <v>570</v>
+      </c>
     </row>
     <row r="41" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>504</v>
+        <v>556</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>351</v>
@@ -3758,10 +4176,16 @@
       <c r="L41" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="M41" t="s">
+        <v>568</v>
+      </c>
+      <c r="N41" t="s">
+        <v>570</v>
+      </c>
     </row>
     <row r="42" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>505</v>
+        <v>557</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>359</v>
@@ -3796,10 +4220,16 @@
       <c r="L42" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="M42" t="s">
+        <v>568</v>
+      </c>
+      <c r="N42" t="s">
+        <v>569</v>
+      </c>
     </row>
     <row r="43" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>506</v>
+        <v>558</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>367</v>
@@ -3834,10 +4264,16 @@
       <c r="L43" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="M43" t="s">
+        <v>568</v>
+      </c>
+      <c r="N43" t="s">
+        <v>569</v>
+      </c>
     </row>
     <row r="44" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>507</v>
+        <v>559</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>376</v>
@@ -3872,10 +4308,16 @@
       <c r="L44" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="M44" t="s">
+        <v>567</v>
+      </c>
+      <c r="N44" t="s">
+        <v>570</v>
+      </c>
     </row>
     <row r="45" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>508</v>
+        <v>560</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>385</v>
@@ -3910,10 +4352,16 @@
       <c r="L45" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="M45" t="s">
+        <v>567</v>
+      </c>
+      <c r="N45" t="s">
+        <v>572</v>
+      </c>
     </row>
     <row r="46" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>509</v>
+        <v>561</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>393</v>
@@ -3948,10 +4396,16 @@
       <c r="L46" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="M46" t="s">
+        <v>567</v>
+      </c>
+      <c r="N46" t="s">
+        <v>570</v>
+      </c>
     </row>
     <row r="47" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>510</v>
+        <v>562</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>401</v>
@@ -3986,10 +4440,16 @@
       <c r="L47" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="M47" t="s">
+        <v>567</v>
+      </c>
+      <c r="N47" t="s">
+        <v>570</v>
+      </c>
     </row>
     <row r="48" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>511</v>
+        <v>563</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>409</v>
@@ -4024,10 +4484,16 @@
       <c r="L48" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="M48" t="s">
+        <v>568</v>
+      </c>
+      <c r="N48" t="s">
+        <v>573</v>
+      </c>
     </row>
     <row r="49" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>512</v>
+        <v>564</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>417</v>
@@ -4062,10 +4528,16 @@
       <c r="L49" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="M49" t="s">
+        <v>568</v>
+      </c>
+      <c r="N49" t="s">
+        <v>570</v>
+      </c>
     </row>
     <row r="50" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>513</v>
+        <v>565</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>426</v>
@@ -4100,10 +4572,16 @@
       <c r="L50" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="M50" t="s">
+        <v>567</v>
+      </c>
+      <c r="N50" t="s">
+        <v>573</v>
+      </c>
     </row>
     <row r="51" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>514</v>
+        <v>566</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>435</v>
@@ -4137,6 +4615,12 @@
       </c>
       <c r="L51" s="5" t="s">
         <v>22</v>
+      </c>
+      <c r="M51" t="s">
+        <v>567</v>
+      </c>
+      <c r="N51" t="s">
+        <v>569</v>
       </c>
     </row>
   </sheetData>

</xml_diff>